<commit_message>
Added excel file classes
</commit_message>
<xml_diff>
--- a/src/main/java/com/test/automation/UIautomation/data/Testdata.xlsx
+++ b/src/main/java/com/test/automation/UIautomation/data/Testdata.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="330" windowWidth="13845" windowHeight="2670"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14895" windowHeight="3945"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestdata" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>Username</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t>aut5@gmail.com</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -142,6 +148,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -189,7 +198,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -224,7 +233,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -436,7 +445,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,6 +472,9 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -471,6 +483,9 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -479,6 +494,9 @@
       <c r="B4" t="s">
         <v>4</v>
       </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -486,6 +504,9 @@
       </c>
       <c r="B5" t="s">
         <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>